<commit_message>
info page V1.1 minor changes+small easter egg
</commit_message>
<xml_diff>
--- a/ignore_pls/Group C WDD_project_task_list.xlsx
+++ b/ignore_pls/Group C WDD_project_task_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentncirl-my.sharepoint.com/personal/x24709515_student_ncirl_ie/Documents/Web-Design-Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentncirl-my.sharepoint.com/personal/x24709515_student_ncirl_ie/Documents/Web-Design-Project/ignore_pls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{79121A4C-96C8-4C6C-B535-2AAE90A8FCE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F21AFD84-D39A-4374-958A-82E3C834637E}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="8_{79121A4C-96C8-4C6C-B535-2AAE90A8FCE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BC71EA4-0E45-4550-8B80-F06A0B07534F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CC4871A7-87E9-400E-8844-9811E13AA789}"/>
+    <workbookView minimized="1" xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{CC4871A7-87E9-400E-8844-9811E13AA789}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
   <si>
     <t>WDD_Project_2024</t>
   </si>
@@ -163,13 +163,19 @@
   </si>
   <si>
     <t>Antonio</t>
+  </si>
+  <si>
+    <t>experiment with layout</t>
+  </si>
+  <si>
+    <t>simplefy/fix code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,9 +251,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -285,7 +291,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -391,7 +397,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -533,7 +539,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -543,20 +549,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89A20EA6-9FE1-4F65-A2C0-41C46F4D1B7C}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="23.45"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="104.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="8.7109375" style="3"/>
+    <col min="1" max="1" width="14.5546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="104.109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="8.6640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="46.9">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="46.8" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -567,7 +573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1">
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -575,12 +581,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
@@ -588,7 +594,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -596,7 +602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
@@ -604,7 +610,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
@@ -612,13 +618,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B9" s="3" t="s">
         <v>12</v>
       </c>
@@ -626,20 +632,26 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="C11" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="C12" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
@@ -647,7 +659,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B14" s="3" t="s">
         <v>17</v>
       </c>
@@ -655,30 +667,42 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B15" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B16" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="C16" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="C19" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B20" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="C20" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B21" s="3" t="s">
         <v>23</v>
       </c>
@@ -686,7 +710,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B22" s="3" t="s">
         <v>24</v>
       </c>
@@ -694,12 +718,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B23" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="C23" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B24" s="3" t="s">
         <v>19</v>
       </c>
@@ -707,20 +734,42 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="C26" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B27" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B29" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="C29" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>27</v>
       </c>
@@ -728,57 +777,63 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B32" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B33" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B34" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B35" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B36" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B37" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B38" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B39" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B40" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="C40" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B41" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="C41" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
         <v>39</v>
       </c>
@@ -786,7 +841,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B45" s="3" t="s">
         <v>41</v>
       </c>
@@ -798,55 +853,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <DefaultSectionNames xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
-    <Invited_Teachers xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
-    <Owner xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Has_Teacher_Only_SectionGroup xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
-    <Invited_Students xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
-    <CultureName xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
-    <Distribution_Groups xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
-    <TeamsChannelId xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
-    <Teachers xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <Math_Settings xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
-    <FolderType xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
-    <Templates xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
-    <Teams_Channel_Section_Location xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
-    <AppVersion xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
-    <LMS_Mappings xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
-    <NotebookType xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
-    <Students xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <Student_Groups xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1253,22 +1265,90 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <DefaultSectionNames xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
+    <Invited_Teachers xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
+    <Owner xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Has_Teacher_Only_SectionGroup xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
+    <Invited_Students xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
+    <CultureName xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
+    <Distribution_Groups xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
+    <TeamsChannelId xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
+    <Teachers xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <Math_Settings xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
+    <FolderType xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
+    <Templates xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
+    <Teams_Channel_Section_Location xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
+    <AppVersion xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
+    <LMS_Mappings xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
+    <NotebookType xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044" xsi:nil="true"/>
+    <Students xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <Student_Groups xmlns="a400bed3-dd80-47b5-be8a-0e5cea58c044">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45813AF1-8288-45E9-83B6-FF3A559347C4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8144FC7C-9872-4D39-8984-1737A434D946}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4A6CF24-95A3-4D7A-A7CF-B44ADA1363FA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4A6CF24-95A3-4D7A-A7CF-B44ADA1363FA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a400bed3-dd80-47b5-be8a-0e5cea58c044"/>
+    <ds:schemaRef ds:uri="bf565209-2b21-4ee4-af8d-f3a2c0cda902"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8144FC7C-9872-4D39-8984-1737A434D946}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45813AF1-8288-45E9-83B6-FF3A559347C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a400bed3-dd80-47b5-be8a-0e5cea58c044"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>